<commit_message>
Changed TS colour for harvard dataset
</commit_message>
<xml_diff>
--- a/harvard-clean-energy/Harvard summary statistics.xlsx
+++ b/harvard-clean-energy/Harvard summary statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rubai\Documents\Programming\AI3SD\edbo\harvard-clean-energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71512393-A2C9-4CF2-A0A6-99F0488632D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8415698-A241-4305-93DA-8CD54B09E9C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,36 +18,32 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$2:$B$51</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$C$2:$C$51</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$D$2:$D$51</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$B$2:$B$51</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$2:$C$51</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$A$2:$A$51</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$B$2:$B$51</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$C$2:$C$51</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$D$2:$D$51</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$C$2:$C$51</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$D$2:$D$51</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$B$2:$B$51</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$C$2:$C$51</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$A$2:$A$51</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$B$2:$B$51</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$C$2:$C$51</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$D$2:$D$51</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$51</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$D$2:$D$51</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$2:$C$51</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$D$2:$D$51</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$A$2:$A$51</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$A$2:$A$51</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$2:$B$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -125,6 +121,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF4361EE"/>
       <color rgb="FF4CC9F0"/>
       <color rgb="FF3A0CA3"/>
       <color rgb="FF7209B7"/>
@@ -147,32 +144,27 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.25</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.27</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.29</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="3">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.31</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{B847D395-372E-4B51-9721-B3CBFB2A0877}">
+        <cx:series layoutId="boxWhisker" uniqueId="{B847D395-372E-4B51-9721-B3CBFB2A0877}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.24</cx:f>
+              <cx:f>_xlchart.v1.12</cx:f>
               <cx:v>Random</cx:v>
             </cx:txData>
           </cx:tx>
@@ -192,10 +184,10 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{5840D0DF-CEE3-43EF-A0CD-4F7E97473CAD}">
+        <cx:series layoutId="boxWhisker" uniqueId="{5840D0DF-CEE3-43EF-A0CD-4F7E97473CAD}" formatIdx="1">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.26</cx:f>
+              <cx:f>_xlchart.v1.14</cx:f>
               <cx:v>EI</cx:v>
             </cx:txData>
           </cx:tx>
@@ -215,16 +207,16 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{A7490D36-6268-48CC-974C-6221A6FDB6F8}">
+        <cx:series layoutId="boxWhisker" uniqueId="{A7490D36-6268-48CC-974C-6221A6FDB6F8}" formatIdx="2">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.28</cx:f>
+              <cx:f>_xlchart.v1.16</cx:f>
               <cx:v>TS</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
             <a:solidFill>
-              <a:srgbClr val="3A0CA3"/>
+              <a:srgbClr val="4361EE"/>
             </a:solidFill>
             <a:ln>
               <a:solidFill>
@@ -238,29 +230,6 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{A519D200-F837-4BD1-9FD0-C4CD967F21A0}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.30</cx:f>
-              <cx:v>EI-TS</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4CC9F0"/>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-          </cx:spPr>
-          <cx:dataId val="3"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
       </cx:plotAreaRegion>
       <cx:axis id="0" hidden="1">
         <cx:catScaling gapWidth="1"/>
@@ -268,34 +237,6 @@
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling max="11.5" min="9"/>
-        <cx:title>
-          <cx:tx>
-            <cx:txData>
-              <cx:v>Max observed PCE</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:txPr>
-            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:sysClr>
-                  </a:solidFill>
-                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-                </a:rPr>
-                <a:t>Max observed PCE</a:t>
-              </a:r>
-            </a:p>
-          </cx:txPr>
-        </cx:title>
         <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
@@ -865,15 +806,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -909,8 +850,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4800600" y="5166360"/>
-              <a:ext cx="2811780" cy="5036820"/>
+              <a:off x="4869180" y="6385560"/>
+              <a:ext cx="2811780" cy="4061460"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1208,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="P50" sqref="P50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>